<commit_message>
beta V2.1 add env file
</commit_message>
<xml_diff>
--- a/Welocme.xlsx
+++ b/Welocme.xlsx
@@ -14,24 +14,72 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="27">
   <si>
     <t>Resources table</t>
   </si>
   <si>
-    <t>name</t>
-  </si>
-  <si>
-    <t>type</t>
-  </si>
-  <si>
-    <t>sources</t>
-  </si>
-  <si>
-    <t>transformations</t>
-  </si>
-  <si>
-    <t>RQ</t>
+    <t>[</t>
+  </si>
+  <si>
+    <t>'</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>e</t>
+  </si>
+  <si>
+    <t>,</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>t</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>o</t>
+  </si>
+  <si>
+    <t>u</t>
+  </si>
+  <si>
+    <t>r</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>i</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>Q</t>
+  </si>
+  <si>
+    <t>]</t>
   </si>
   <si>
     <t>employee_id</t>
@@ -44,6 +92,9 @@
   </si>
   <si>
     <t>object</t>
+  </si>
+  <si>
+    <t>CodeSpeedy</t>
   </si>
 </sst>
 </file>
@@ -386,7 +437,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:BA4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -395,12 +446,12 @@
     <col min="1" max="5" width="50.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:53">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:53">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -416,21 +467,171 @@
       <c r="E2" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="F2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="W2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="X2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="Y2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="Z2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AA2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AB2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="AC2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AD2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="AE2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="AF2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="AG2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="AH2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="AI2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="AJ2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="AK2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="AL2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="AM2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="AN2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="AO2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="AP2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="AQ2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="AR2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="AS2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AT2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AU2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="AV2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AW2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="AX2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="AY2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AZ2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="BA2" s="1" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:53">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>24</v>
+      </c>
+      <c r="C3" t="s">
+        <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:53">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>25</v>
+      </c>
+      <c r="C4" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>